<commit_message>
fixed some formatting and linted problems.
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">CVNA</t>
   </si>
   <si>
+    <t xml:space="preserve">DBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMB</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t xml:space="preserve">LPG</t>
   </si>
   <si>
+    <t xml:space="preserve">MXEA</t>
+  </si>
+  <si>
     <t xml:space="preserve">NG</t>
   </si>
   <si>
@@ -113,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">ROKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM</t>
   </si>
   <si>
     <t xml:space="preserve">RUT</t>
@@ -249,13 +261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
@@ -328,7 +340,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.175</v>
+        <v>0.911</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,7 +348,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,7 +356,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.877</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,7 +364,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.417</v>
+        <v>0.877</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,7 +372,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.114</v>
+        <v>0.417</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,7 +380,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.896</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,18 +388,18 @@
         <v>16</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>17</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>0.289</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +407,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.457</v>
+        <v>0.289</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,7 +415,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.703</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,18 +423,18 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.252</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>22</v>
+        <v>0.703</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0.906</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,8 +442,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="0" t="n">
-        <f aca="false">B27</f>
-        <v>0.869</v>
+        <v>0.906</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +450,8 @@
         <v>25</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.2</v>
+        <f aca="false">B31</f>
+        <v>0.869</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,7 +459,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.837</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +467,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.024</v>
+        <v>0.837</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,15 +475,15 @@
         <v>28</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.789</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>0.649</v>
+      <c r="B25" s="0" t="n">
+        <v>0.024</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,15 +491,15 @@
         <v>30</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.633</v>
+        <v>0.789</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>0.869</v>
+      <c r="B27" s="1" t="n">
+        <v>0.649</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,56 +507,53 @@
         <v>32</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.264</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>33</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>35</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>33</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>1.43</v>
+        <v>0.869</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.302</v>
+        <v>0.264</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>0.135</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,7 +561,10 @@
         <v>40</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.146</v>
+        <v>0.55</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,7 +572,7 @@
         <v>41</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,6 +580,38 @@
         <v>42</v>
       </c>
       <c r="B36" s="0" t="n">
+        <v>0.302</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.135</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.146</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="0" t="n">
         <v>-0.534</v>
       </c>
     </row>

</xml_diff>

<commit_message>
seemed to be a lot of problems with reading the csv. The internet thinks that the solution is pandas (whatever they are).
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">DBA</t>
   </si>
   <si>
+    <t xml:space="preserve">DJ600</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMB</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">GDX</t>
   </si>
   <si>
+    <t xml:space="preserve">GLEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">GDXJ</t>
   </si>
   <si>
@@ -115,6 +121,12 @@
     <t xml:space="preserve">QQQ</t>
   </si>
   <si>
+    <t xml:space="preserve">PAAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basically SLV</t>
+  </si>
+  <si>
     <t xml:space="preserve">RACE</t>
   </si>
   <si>
@@ -139,7 +151,10 @@
     <t xml:space="preserve">SI</t>
   </si>
   <si>
-    <t xml:space="preserve">unicorn bay, but very term depended. back to 2014 it drops to .1</t>
+    <t xml:space="preserve">unicorn bay, but very term dependent. back to 2014 it drops to .1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLV</t>
   </si>
   <si>
     <t xml:space="preserve">STNG</t>
@@ -261,10 +276,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,7 +363,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.175</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +371,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +379,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.877</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +387,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.417</v>
+        <v>0.877</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +395,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.114</v>
+        <v>0.417</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +403,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.896</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,18 +411,18 @@
         <v>17</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>0.289</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,7 +430,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.457</v>
+        <v>0.289</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,7 +438,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.703</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,27 +446,26 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.252</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>23</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.906</v>
+        <v>0.703</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <f aca="false">B31</f>
-        <v>0.869</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +473,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.2</v>
+        <v>0.906</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,7 +481,8 @@
         <v>27</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.837</v>
+        <f aca="false">B34</f>
+        <v>0.869</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,7 +490,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.66</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,7 +498,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.024</v>
+        <v>0.837</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,15 +506,15 @@
         <v>30</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.789</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>0.649</v>
+      <c r="B27" s="0" t="n">
+        <v>0.024</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,7 +522,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.633</v>
+        <v>0.789</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,34 +530,34 @@
         <v>33</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.34</v>
+        <v>0.123</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0.75</v>
+        <v>35</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0.649</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.869</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.264</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>37</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,29 +565,26 @@
         <v>38</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>39</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>37</v>
+        <v>0.869</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>1.43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,38 +592,77 @@
         <v>42</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.302</v>
+        <v>0.1</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.135</v>
+        <f aca="false">B36</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.146</v>
+        <v>0.55</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="n">
+        <v>0.302</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.135</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.146</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="0" t="n">
         <v>-0.534</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some considerable problems reading csv output from TWS, and reading spreadsheets. You may need pandas.
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -76,6 +76,12 @@
     <t xml:space="preserve">FTMIB</t>
   </si>
   <si>
+    <t xml:space="preserve">GBP.JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBJP not right but value in JPY which is too big</t>
+  </si>
+  <si>
     <t xml:space="preserve">GC</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t xml:space="preserve">GDX</t>
   </si>
   <si>
+    <t xml:space="preserve">GLD</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLEN</t>
   </si>
   <si>
@@ -100,6 +109,12 @@
     <t xml:space="preserve">xx</t>
   </si>
   <si>
+    <t xml:space="preserve">HG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spy vs jjc</t>
+  </si>
+  <si>
     <t xml:space="preserve">HYG</t>
   </si>
   <si>
@@ -142,6 +157,9 @@
     <t xml:space="preserve">RUT</t>
   </si>
   <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHOP</t>
   </si>
   <si>
@@ -157,6 +175,9 @@
     <t xml:space="preserve">SLV</t>
   </si>
   <si>
+    <t xml:space="preserve">SPCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">STNG</t>
   </si>
   <si>
@@ -164,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">TSLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALE</t>
   </si>
   <si>
     <t xml:space="preserve">VNQ</t>
@@ -276,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
@@ -419,7 +443,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.02</v>
+        <v>-0.0061</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>19</v>
@@ -430,42 +454,42 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.289</v>
+        <v>0.02</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.457</v>
+        <v>0.289</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.38</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.703</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.252</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,7 +497,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.906</v>
+        <v>0.703</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,121 +505,121 @@
         <v>27</v>
       </c>
       <c r="B23" s="0" t="n">
-        <f aca="false">B34</f>
-        <v>0.869</v>
+        <v>0.252</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.2</v>
+        <v>0.72</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.837</v>
+        <v>0.906</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.66</v>
+        <f aca="false">B37</f>
+        <v>0.869</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.024</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.789</v>
+        <v>0.837</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.123</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>34</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>0.649</v>
+        <v>36</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.024</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.633</v>
+        <v>0.789</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.34</v>
+        <v>0.123</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>0.75</v>
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0.649</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.869</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.264</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>41</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>43</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,8 +627,7 @@
         <v>44</v>
       </c>
       <c r="B37" s="0" t="n">
-        <f aca="false">B36</f>
-        <v>0.1</v>
+        <v>0.869</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,10 +635,7 @@
         <v>45</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>41</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,46 +643,104 @@
         <v>46</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1.43</v>
+        <v>0.264</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.302</v>
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.135</v>
+        <f aca="false">B40</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>0.146</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0</v>
+        <v>0.55</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B44" s="0" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.302</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.135</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.146</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="0" t="n">
         <v>-0.534</v>
       </c>
     </row>

</xml_diff>

<commit_message>
slight tweaks. Still problems with reading betas which are formulae.
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -303,7 +303,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,7 +544,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.2</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,7 +665,6 @@
         <v>50</v>
       </c>
       <c r="B41" s="0" t="n">
-        <f aca="false">B40</f>
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
can exclude some sec. types now.
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -28,27 +28,60 @@
     <t xml:space="preserve"> Beta</t>
   </si>
   <si>
-    <t xml:space="preserve">ImpVol</t>
+    <t xml:space="preserve">SecType</t>
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIGCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weird, huh?</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGG</t>
   </si>
   <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
     <t xml:space="preserve">BKLN</t>
   </si>
   <si>
     <t xml:space="preserve">BNDX</t>
   </si>
   <si>
+    <t xml:space="preserve">BRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set to be same as MXN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BTP</t>
   </si>
   <si>
+    <t xml:space="preserve">CAD</t>
+  </si>
+  <si>
     <t xml:space="preserve">CL</t>
   </si>
   <si>
+    <t xml:space="preserve">CMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">CVNA</t>
   </si>
   <si>
@@ -58,18 +91,30 @@
     <t xml:space="preserve">DJ600</t>
   </si>
   <si>
+    <t xml:space="preserve">DX</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMB</t>
   </si>
   <si>
+    <t xml:space="preserve">CRE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ES</t>
   </si>
   <si>
     <t xml:space="preserve">ESTX50</t>
   </si>
   <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
     <t xml:space="preserve">EURN</t>
   </si>
   <si>
+    <t xml:space="preserve">EWZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">FRO</t>
   </si>
   <si>
@@ -106,9 +151,6 @@
     <t xml:space="preserve">HCC</t>
   </si>
   <si>
-    <t xml:space="preserve">xx</t>
-  </si>
-  <si>
     <t xml:space="preserve">HG</t>
   </si>
   <si>
@@ -127,12 +169,21 @@
     <t xml:space="preserve">LPG</t>
   </si>
   <si>
+    <t xml:space="preserve">LTAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used ILF</t>
+  </si>
+  <si>
     <t xml:space="preserve">MXEA</t>
   </si>
   <si>
     <t xml:space="preserve">NG</t>
   </si>
   <si>
+    <t xml:space="preserve">NQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">QQQ</t>
   </si>
   <si>
@@ -142,9 +193,18 @@
     <t xml:space="preserve">basically SLV</t>
   </si>
   <si>
+    <t xml:space="preserve">PCY</t>
+  </si>
+  <si>
     <t xml:space="preserve">RACE</t>
   </si>
   <si>
+    <t xml:space="preserve">RDXUSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEP!</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROKU</t>
   </si>
   <si>
@@ -154,6 +214,9 @@
     <t xml:space="preserve">REM</t>
   </si>
   <si>
+    <t xml:space="preserve">RUR</t>
+  </si>
+  <si>
     <t xml:space="preserve">RUT</t>
   </si>
   <si>
@@ -163,9 +226,6 @@
     <t xml:space="preserve">SHOP</t>
   </si>
   <si>
-    <t xml:space="preserve">xxx</t>
-  </si>
-  <si>
     <t xml:space="preserve">SI</t>
   </si>
   <si>
@@ -178,22 +238,37 @@
     <t xml:space="preserve">SPCE</t>
   </si>
   <si>
+    <t xml:space="preserve">SPY</t>
+  </si>
+  <si>
     <t xml:space="preserve">STNG</t>
   </si>
   <si>
     <t xml:space="preserve">SX7P</t>
   </si>
   <si>
+    <t xml:space="preserve">TLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TNK</t>
+  </si>
+  <si>
     <t xml:space="preserve">TSLA</t>
   </si>
   <si>
     <t xml:space="preserve">VALE</t>
   </si>
   <si>
+    <t xml:space="preserve">VIX</t>
+  </si>
+  <si>
     <t xml:space="preserve">VNQ</t>
   </si>
   <si>
     <t xml:space="preserve">XLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
   </si>
   <si>
     <t xml:space="preserve">ZAR</t>
@@ -206,8 +281,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -274,8 +351,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,16 +385,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,416 +416,776 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.523</v>
+        <v>-1.254</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.829</v>
+        <v>0.93</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.428</v>
+        <v>0.523</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.259</v>
+        <v>0.829</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.53</v>
+        <v>0.428</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.53</v>
+        <v>-1.26</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.259</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.911</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.75</v>
+        <v>-1.98</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.175</v>
+        <v>0.53</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>0.41</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>10000000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.877</v>
+        <v>0.53</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>2000000000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.417</v>
+        <v>0.911</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">H11/H12</f>
+        <v>0.005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.114</v>
+        <v>0.75</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.896</v>
+        <v>0.45</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-0.0061</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>19</v>
+        <v>0.175</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.289</v>
+        <v>0.877</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.457</v>
+        <v>0.6</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.02</v>
+        <v>0.417</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.38</v>
+        <v>0.44</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.703</v>
+        <v>0.114</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.252</v>
+        <v>0.896</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.72</v>
+        <v>-0.0061</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.906</v>
+        <v>0.02</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="n">
-        <f aca="false">B37</f>
-        <v>0.869</v>
+        <v>0.289</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.001</v>
+        <v>0.457</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.837</v>
+        <v>0.02</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.66</v>
+        <v>0.38</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.024</v>
+        <v>0.703</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.789</v>
+        <v>0.252</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.123</v>
+        <v>0.72</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>0.649</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.633</v>
+        <v>0.87</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.34</v>
+        <v>0.001</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>0.008</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.75</v>
+        <v>0.837</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.869</v>
+        <v>0.55</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.081</v>
+        <v>0.66</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.264</v>
+        <v>0.024</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>49</v>
+        <v>0.79</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.1</v>
+        <v>0.789</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2</v>
+        <v>0.123</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0.55</v>
+        <v>0.85</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>1.43</v>
+        <v>58</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>0.302</v>
+        <v>59</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0.43</v>
+        <v>0.633</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0.135</v>
+        <v>0.34</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0.146</v>
+        <v>0.75</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>0</v>
+        <v>-1.125</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B50" s="0" t="n">
+        <v>0.869</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>-0.67</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>0.302</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>-0.266</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>-1.122</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="0" t="n">
         <v>-0.534</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest changes, not sure what
</commit_message>
<xml_diff>
--- a/betavals.xlsx
+++ b/betavals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -34,27 +34,33 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">AEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIGCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weird, huh?</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUD</t>
   </si>
   <si>
     <t xml:space="preserve">FX</t>
   </si>
   <si>
-    <t xml:space="preserve">AIGCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weird, huh?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
     <t xml:space="preserve">BKLN</t>
   </si>
   <si>
@@ -79,9 +85,6 @@
     <t xml:space="preserve">CMG</t>
   </si>
   <si>
-    <t xml:space="preserve">EQ</t>
-  </si>
-  <si>
     <t xml:space="preserve">CVNA</t>
   </si>
   <si>
@@ -112,6 +115,12 @@
     <t xml:space="preserve">EURN</t>
   </si>
   <si>
+    <t xml:space="preserve">EWA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EWT</t>
+  </si>
+  <si>
     <t xml:space="preserve">EWZ</t>
   </si>
   <si>
@@ -121,6 +130,9 @@
     <t xml:space="preserve">FTMIB</t>
   </si>
   <si>
+    <t xml:space="preserve">FXI</t>
+  </si>
+  <si>
     <t xml:space="preserve">GBP.JPY</t>
   </si>
   <si>
@@ -139,15 +151,15 @@
     <t xml:space="preserve">GDX</t>
   </si>
   <si>
+    <t xml:space="preserve">GDXJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLD</t>
   </si>
   <si>
     <t xml:space="preserve">GLEN</t>
   </si>
   <si>
-    <t xml:space="preserve">GDXJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">HCC</t>
   </si>
   <si>
@@ -160,9 +172,24 @@
     <t xml:space="preserve">HYG</t>
   </si>
   <si>
+    <t xml:space="preserve">IBEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">based on ief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILF</t>
+  </si>
+  <si>
     <t xml:space="preserve">IWM</t>
   </si>
   <si>
+    <t xml:space="preserve">KL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LK</t>
   </si>
   <si>
@@ -178,40 +205,52 @@
     <t xml:space="preserve">MXEA</t>
   </si>
   <si>
+    <t xml:space="preserve">NAV</t>
+  </si>
+  <si>
     <t xml:space="preserve">NG</t>
   </si>
   <si>
+    <t xml:space="preserve">NKLA</t>
+  </si>
+  <si>
     <t xml:space="preserve">NQ</t>
   </si>
   <si>
+    <t xml:space="preserve">PAAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basically SLV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCY</t>
+  </si>
+  <si>
     <t xml:space="preserve">QQQ</t>
   </si>
   <si>
-    <t xml:space="preserve">PAAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basically SLV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCY</t>
-  </si>
-  <si>
     <t xml:space="preserve">RACE</t>
   </si>
   <si>
+    <t xml:space="preserve">RDSA</t>
+  </si>
+  <si>
     <t xml:space="preserve">RDXUSD</t>
   </si>
   <si>
     <t xml:space="preserve">YEP!</t>
   </si>
   <si>
+    <t xml:space="preserve">REM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIG</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROKU</t>
   </si>
   <si>
-    <t xml:space="preserve">RDSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REM</t>
+    <t xml:space="preserve">RRC</t>
   </si>
   <si>
     <t xml:space="preserve">RUR</t>
@@ -265,6 +304,12 @@
     <t xml:space="preserve">VNQ</t>
   </si>
   <si>
+    <t xml:space="preserve">VWO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
     <t xml:space="preserve">XLF</t>
   </si>
   <si>
@@ -272,6 +317,9 @@
   </si>
   <si>
     <t xml:space="preserve">ZAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZI</t>
   </si>
   <si>
     <t xml:space="preserve">ZM</t>
@@ -351,7 +399,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,6 +409,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,13 +437,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -416,7 +468,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-1.254</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
@@ -427,23 +479,23 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.93</v>
+        <v>0.523</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.523</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -452,35 +504,32 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.829</v>
+        <v>-1.254</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.428</v>
+        <v>0.829</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-1.26</v>
+        <v>0.428</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,43 +537,46 @@
         <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.259</v>
+        <v>-1.26</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>-1.98</v>
+        <v>0.259</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.53</v>
+        <v>-1.98</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.41</v>
+        <v>0.53</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>10000000000</v>
@@ -535,10 +587,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>2000000000000</v>
@@ -549,10 +601,10 @@
         <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.911</v>
+        <v>0.53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">H11/H12</f>
@@ -564,10 +616,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.75</v>
+        <v>0.911</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>5</v>
@@ -586,21 +638,21 @@
         <v>24</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.175</v>
+        <v>0.45</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,10 +660,10 @@
         <v>27</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.877</v>
+        <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +671,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.6</v>
+        <v>0.877</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>5</v>
@@ -630,10 +682,10 @@
         <v>29</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.417</v>
+        <v>0.6</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,10 +693,10 @@
         <v>30</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.44</v>
+        <v>0.417</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,10 +704,10 @@
         <v>31</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.114</v>
+        <v>0.637</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,10 +715,10 @@
         <v>32</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.896</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>19</v>
+        <v>0.918</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,71 +726,71 @@
         <v>33</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-0.0061</v>
+        <v>0.44</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.02</v>
+        <v>0.114</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.289</v>
+        <v>0.896</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>7</v>
+        <v>0.918</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.02</v>
+        <v>-0.0061</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,10 +798,10 @@
         <v>41</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.703</v>
+        <v>0.289</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,10 +809,10 @@
         <v>42</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.252</v>
+        <v>0.457</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,60 +820,57 @@
         <v>43</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.72</v>
+        <v>0.703</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0.906</v>
+        <v>0.02</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.87</v>
+        <v>0.38</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.001</v>
+        <v>0.252</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K35" s="2" t="n">
-        <v>0.008</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0.837</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,35 +878,38 @@
         <v>49</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.55</v>
+        <v>0.906</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>0.008</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.66</v>
+        <v>0.785</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.024</v>
+        <v>-2.09</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,10 +917,10 @@
         <v>53</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>19</v>
+        <v>0.544</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,10 +928,10 @@
         <v>54</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.789</v>
+        <v>0.87</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,90 +939,87 @@
         <v>55</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>0.123</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>56</v>
+        <v>0.071</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0.85</v>
+        <v>0.001</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="3" t="n">
-        <v>0.649</v>
+        <v>57</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.837</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="B45" s="3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0.633</v>
+        <v>0.66</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>19</v>
+        <v>0.157</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0.75</v>
+        <v>0.024</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>-1.125</v>
+        <v>2</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>5</v>
@@ -978,24 +1027,27 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0.869</v>
+        <v>0.79</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>0.081</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,10 +1055,10 @@
         <v>67</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0.264</v>
+        <v>0.85</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,46 +1066,46 @@
         <v>68</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>0.1</v>
+        <v>0.789</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>0.1</v>
+        <v>69</v>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>0.649</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>2</v>
+        <v>0.34</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,10 +1113,10 @@
         <v>73</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>0.55</v>
+        <v>0.75</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,10 +1124,10 @@
         <v>74</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>1.43</v>
+        <v>0.126</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,10 +1135,10 @@
         <v>75</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>-0.67</v>
+        <v>0.633</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,10 +1146,10 @@
         <v>76</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>0.107</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>19</v>
+        <v>0.113</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,10 +1157,10 @@
         <v>77</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>0.302</v>
+        <v>-1.125</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,10 +1168,10 @@
         <v>78</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>0.43</v>
+        <v>0.869</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,10 +1179,10 @@
         <v>79</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>-0.266</v>
+        <v>0.081</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,10 +1190,10 @@
         <v>80</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>0.135</v>
+        <v>0.264</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,29 +1201,32 @@
         <v>81</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>0.146</v>
+        <v>0.1</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>0.88</v>
+        <v>0.1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>-1.122</v>
+        <v>2</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>5</v>
@@ -1179,13 +1234,178 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>-0.67</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>0.302</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>-0.266</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>0.919</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>0.169</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>-1.122</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>0.0087</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83" s="0" t="n">
         <v>-0.534</v>
       </c>
-      <c r="C68" s="0" t="s">
-        <v>19</v>
+      <c r="C83" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>